<commit_message>
Final commit: bar chart with a twist
</commit_message>
<xml_diff>
--- a/Excel bar charts with a twist data.xlsx
+++ b/Excel bar charts with a twist data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Year</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>% sales to target</t>
+  </si>
+  <si>
+    <t>Formula used</t>
   </si>
 </sst>
 </file>
@@ -382,28 +385,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>27312</c:v>
+                  <c:v>37109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43157</c:v>
+                  <c:v>19752</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19420</c:v>
+                  <c:v>39771</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46280</c:v>
+                  <c:v>16358</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18733</c:v>
+                  <c:v>12617</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12493</c:v>
+                  <c:v>32602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22804</c:v>
+                  <c:v>11538</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24110</c:v>
+                  <c:v>29577</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -626,6 +629,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000"/>
+              <a:t>Sales vs Target per Quarter (2023 - 2024)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -678,15 +706,77 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="10000"/>
+                  <a:alpha val="54000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg2">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>data!$A$2:$B$9</c:f>
@@ -784,14 +874,451 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent2">
+                <a:alpha val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0E27F9F0-A4A4-4D28-A59B-D12A76FED0F1}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{B3169400-61FB-4723-8D39-BD8CF54F60D6}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CABE60C8-22BD-4ACA-A1CE-883B57FF5627}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{7BCCF8AA-4E4D-4EBE-9A72-871AEC099BF0}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{483FB28F-4156-4208-94E0-65B608D64AD5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{E44D0021-9D2D-4D82-BECE-80B28BEFE35E}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F564E6AE-7AD1-4ECC-93C4-CEC3EAD0BAC8}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{29847B10-17D6-43A4-A5A2-172C706BD6F9}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{51F8D310-3ECB-46A6-85A6-ECF09AEBD5D8}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{8CEFBD25-EA8C-452A-8ECD-EEE3533BDE5B}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{7436F629-D4BA-43D7-9E3F-DEFB525510AB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{3845A3B8-B346-41BD-95C2-7BDA2D0CEA36}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{242D1363-F4A3-4209-A8CD-7AE83FA4CEAA}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{9B797F88-DC27-4817-951D-04446DCF5080}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B4A43309-778B-46BB-A833-418956C3D8D2}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                  <a:p>
+                    <a:fld id="{D07784CA-2E81-4525-BF63-539499897293}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+</c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-1186-4E60-A75A-489EC12D301A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent6">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:separator>
+</c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>data!$A$2:$B$9</c:f>
@@ -841,33 +1368,65 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>27312</c:v>
+                  <c:v>37109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43157</c:v>
+                  <c:v>19752</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19420</c:v>
+                  <c:v>39771</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46280</c:v>
+                  <c:v>16358</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18733</c:v>
+                  <c:v>12617</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12493</c:v>
+                  <c:v>32602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22804</c:v>
+                  <c:v>11538</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24110</c:v>
+                  <c:v>29577</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>data!$F$2:$F$9</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>93%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>66%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>159%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>82%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>28%</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>93%</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>38%</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>118%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7B31-479E-B972-965264693760}"/>
             </c:ext>
@@ -881,8 +1440,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="90"/>
+        <c:overlap val="100"/>
         <c:axId val="2125834608"/>
         <c:axId val="2125825040"/>
       </c:barChart>
@@ -915,7 +1474,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -942,53 +1501,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="2125834608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -1002,9 +1520,18 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.0380505715474107E-3"/>
+          <c:y val="0.10617485791375315"/>
+          <c:w val="0.2442189808241183"/>
+          <c:h val="0.11492830571751052"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1017,7 +1544,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2197,16 +2724,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323851</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2493,18 +3020,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="D2" sqref="C2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2520,8 +3049,11 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2023</v>
       </c>
@@ -2532,15 +3064,18 @@
         <v>40000</v>
       </c>
       <c r="D2">
-        <f ca="1">RANDBETWEEN(10000, 50000)</f>
-        <v>27312</v>
+        <v>37109</v>
       </c>
       <c r="F2" t="str">
-        <f ca="1">TEXT(D2/C2,"0.#%")</f>
-        <v>68.3%</v>
+        <f>TEXT(D2/C2,"0%")</f>
+        <v>93%</v>
+      </c>
+      <c r="G2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(F2)</f>
+        <v>=TEXT(D2/C2,"0%")</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>5</v>
@@ -2549,15 +3084,18 @@
         <v>30000</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" ca="1" si="0">RANDBETWEEN(10000, 50000)</f>
-        <v>43157</v>
+        <v>19752</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F9" ca="1" si="1">TEXT(D3/C3,"0.#%")</f>
-        <v>143.9%</v>
+        <f t="shared" ref="F3:F9" si="0">TEXT(D3/C3,"0%")</f>
+        <v>66%</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G9" ca="1" si="1">_xlfn.FORMULATEXT(F3)</f>
+        <v>=TEXT(D3/C3,"0%")</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>6</v>
@@ -2566,15 +3104,18 @@
         <v>25000</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="0"/>
-        <v>19420</v>
+        <v>39771</v>
       </c>
       <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>159%</v>
+      </c>
+      <c r="G4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>77.7%</v>
+        <v>=TEXT(D4/C4,"0%")</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>7</v>
@@ -2583,15 +3124,18 @@
         <v>20000</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="0"/>
-        <v>46280</v>
+        <v>16358</v>
       </c>
       <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>82%</v>
+      </c>
+      <c r="G5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>231.4%</v>
+        <v>=TEXT(D5/C5,"0%")</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2024</v>
       </c>
@@ -2603,15 +3147,18 @@
         <v>45000</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="0"/>
-        <v>18733</v>
+        <v>12617</v>
       </c>
       <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>28%</v>
+      </c>
+      <c r="G6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>41.6%</v>
+        <v>=TEXT(D6/C6,"0%")</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>5</v>
@@ -2621,15 +3168,18 @@
         <v>35000</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="0"/>
-        <v>12493</v>
+        <v>32602</v>
       </c>
       <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>93%</v>
+      </c>
+      <c r="G7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>35.7%</v>
+        <v>=TEXT(D7/C7,"0%")</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>6</v>
@@ -2639,15 +3189,18 @@
         <v>30000</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="0"/>
-        <v>22804</v>
+        <v>11538</v>
       </c>
       <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>38%</v>
+      </c>
+      <c r="G8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>76.%</v>
+        <v>=TEXT(D8/C8,"0%")</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>7</v>
@@ -2657,12 +3210,15 @@
         <v>25000</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="0"/>
-        <v>24110</v>
+        <v>29577</v>
       </c>
       <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>118%</v>
+      </c>
+      <c r="G9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>96.4%</v>
+        <v>=TEXT(D9/C9,"0%")</v>
       </c>
     </row>
   </sheetData>
@@ -2678,8 +3234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2691,30 +3247,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="M3:O4"/>
+  <dimension ref="R3:T4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" topLeftCell="E3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="13:15" x14ac:dyDescent="0.25">
-      <c r="M3" t="s">
+    <row r="3" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="13:15" x14ac:dyDescent="0.25">
-      <c r="M4" t="s">
+    <row r="4" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
         <v>9</v>
       </c>
-      <c r="N4" t="s">
+      <c r="S4" t="s">
         <v>10</v>
       </c>
-      <c r="O4" t="s">
+      <c r="T4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>